<commit_message>
level change msgs tidy up
</commit_message>
<xml_diff>
--- a/game_template/model/data/floor builder Level 9.xlsx
+++ b/game_template/model/data/floor builder Level 9.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Reverser" sheetId="33" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="229">
   <si>
     <t>width</t>
   </si>
@@ -8431,10 +8431,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB1:AB20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10193,16 +10193,6 @@
       </c>
       <c r="B27" s="1">
         <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -12038,7 +12028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>

</xml_diff>